<commit_message>
sample tweets to train
</commit_message>
<xml_diff>
--- a/sentiment analysis/TWEETS.xlsx
+++ b/sentiment analysis/TWEETS.xlsx
@@ -1399,9 +1399,6 @@
     <t>Last week of september. Can say official end of rainy season and hot humid weather in delhi ! Next 5 months will be best time in delhi</t>
   </si>
   <si>
-    <t>Flight to Mumbai from Goa delayed cause of bad weather in Delhi. Talk about irony...</t>
-  </si>
-  <si>
     <t>Such a beautiful weather in Delhi and I am concentrating on Telengana. Sigh.</t>
   </si>
   <si>
@@ -1430,6 +1427,9 @@
   </si>
   <si>
     <t>Pretty cool weather in Delhi today. Meanwhile, I uploaded awesomesauce pic last night. If you havenâ€™t already, See! facebook.com/photo.php?fbidâ€¦</t>
+  </si>
+  <si>
+    <t>Flight to Mumbai from Goa delayed cause of bad weather in Delhi. Talk about irony…</t>
   </si>
 </sst>
 </file>
@@ -1773,8 +1773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A497"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A377" workbookViewId="0">
-      <selection activeCell="A377" sqref="A377"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="A96" sqref="A96:A97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4214,57 +4214,57 @@
     </row>
     <row r="487" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A487" t="s">
-        <v>461</v>
+        <v>471</v>
       </c>
     </row>
     <row r="488" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A488" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="489" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A489" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="490" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A490" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="491" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A491" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="492" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A492" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="493" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A493" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="494" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A494" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="495" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A495" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="496" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A496" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="497" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A497" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
   </sheetData>

</xml_diff>